<commit_message>
added plot_empty_diagonals, to plot the standards that didnt show significant increases
</commit_message>
<xml_diff>
--- a/fig1/Supplements1.xlsx
+++ b/fig1/Supplements1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QTOF\MethodPaper\fig1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3392E70-16DA-4562-B832-B9C79C36F4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E511D8D-3443-48C4-B79C-9AD9EBFAD41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytical_Standards" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -4339,10 +4339,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4625,8 +4625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5411,7 +5411,7 @@
         <v>1</v>
       </c>
       <c r="AG6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(AF6=1,AJ6,AI6)</f>
         <v>trp-L[M+H]+</v>
       </c>
       <c r="AH6" s="25">
@@ -5947,7 +5947,7 @@
         <v>4.5755396287649797</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="11"/>
+        <f>IF(AD10&gt;AE10,1,0)</f>
         <v>1</v>
       </c>
       <c r="AG10" t="str">
@@ -25901,7 +25901,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:155" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30"/>
+      <c r="A1" s="29"/>
       <c r="B1" s="15" t="s">
         <v>168</v>
       </c>
@@ -98464,7 +98464,7 @@
       <c r="F5" s="27">
         <v>0</v>
       </c>
-      <c r="G5" s="29" t="str">
+      <c r="G5" s="30" t="str">
         <f>VLOOKUP(A5,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Amino Acid Metabolism</v>
       </c>
@@ -98498,7 +98498,7 @@
       <c r="F6" s="27">
         <v>0</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="30"/>
       <c r="J6" t="str">
         <v>Cofactor Metabolism</v>
       </c>
@@ -98563,7 +98563,7 @@
       <c r="F8" s="27">
         <v>0</v>
       </c>
-      <c r="G8" s="29" t="str">
+      <c r="G8" s="30" t="str">
         <f>VLOOKUP(A8,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Amino Acid Metabolism</v>
       </c>
@@ -98597,7 +98597,7 @@
       <c r="F9" s="27">
         <v>0</v>
       </c>
-      <c r="G9" s="29"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
@@ -98702,7 +98702,7 @@
       <c r="F13" s="27">
         <v>0</v>
       </c>
-      <c r="G13" s="29" t="str">
+      <c r="G13" s="30" t="str">
         <f>VLOOKUP(A13,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Amino Acid Metabolism</v>
       </c>
@@ -98729,7 +98729,7 @@
       <c r="F14" s="27">
         <v>0</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
@@ -98805,7 +98805,7 @@
       <c r="F17" s="27">
         <v>1</v>
       </c>
-      <c r="G17" s="29" t="str">
+      <c r="G17" s="30" t="str">
         <f>VLOOKUP(A17,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Nucleotide Metabolism</v>
       </c>
@@ -98831,7 +98831,7 @@
       <c r="F18" s="27">
         <v>0</v>
       </c>
-      <c r="G18" s="29"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -98960,7 +98960,7 @@
       <c r="F23" s="27">
         <v>1</v>
       </c>
-      <c r="G23" s="29" t="str">
+      <c r="G23" s="30" t="str">
         <f>VLOOKUP(A23,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Nucleotide Metabolism</v>
       </c>
@@ -98986,7 +98986,7 @@
       <c r="F24" s="27">
         <v>1</v>
       </c>
-      <c r="G24" s="29"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="27" t="s">
@@ -99035,7 +99035,7 @@
       <c r="F26" s="27">
         <v>0</v>
       </c>
-      <c r="G26" s="29" t="str">
+      <c r="G26" s="30" t="str">
         <f>VLOOKUP(A26,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Nucleotide Metabolism</v>
       </c>
@@ -99061,7 +99061,7 @@
       <c r="F27" s="27">
         <v>0</v>
       </c>
-      <c r="G27" s="29"/>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="27" t="s">
@@ -99085,7 +99085,7 @@
       <c r="F28" s="27">
         <v>0</v>
       </c>
-      <c r="G28" s="29" t="str">
+      <c r="G28" s="30" t="str">
         <f>VLOOKUP(A28,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Nucleotide Metabolism</v>
       </c>
@@ -99111,7 +99111,7 @@
       <c r="F29" s="27">
         <v>0</v>
       </c>
-      <c r="G29" s="29"/>
+      <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -99189,7 +99189,7 @@
       <c r="F32" s="27">
         <v>1</v>
       </c>
-      <c r="G32" s="29" t="str">
+      <c r="G32" s="30" t="str">
         <f>VLOOKUP(A32,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Cofactor Metabolism</v>
       </c>
@@ -99216,7 +99216,7 @@
       <c r="F33" s="27">
         <v>1</v>
       </c>
-      <c r="G33" s="29"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="27" t="s">
@@ -99267,7 +99267,7 @@
       <c r="F35" s="27">
         <v>0</v>
       </c>
-      <c r="G35" s="29" t="str">
+      <c r="G35" s="30" t="str">
         <f>VLOOKUP(A35,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Amino Acid Metabolism</v>
       </c>
@@ -99294,7 +99294,7 @@
       <c r="F36" s="27">
         <v>0</v>
       </c>
-      <c r="G36" s="29"/>
+      <c r="G36" s="30"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="27" t="s">
@@ -99344,7 +99344,7 @@
       <c r="F38" s="27">
         <v>0</v>
       </c>
-      <c r="G38" s="29" t="str">
+      <c r="G38" s="30" t="str">
         <f>VLOOKUP(A38,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Amino Acid Metabolism</v>
       </c>
@@ -99370,7 +99370,7 @@
       <c r="F39" s="27">
         <v>0</v>
       </c>
-      <c r="G39" s="29"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -99393,7 +99393,7 @@
       <c r="F40" s="27">
         <v>0</v>
       </c>
-      <c r="G40" s="29"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="27" t="s">
@@ -99416,7 +99416,7 @@
       <c r="F41" s="27">
         <v>0</v>
       </c>
-      <c r="G41" s="29" t="str">
+      <c r="G41" s="30" t="str">
         <f>VLOOKUP(A41,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Cofactor Metabolism</v>
       </c>
@@ -99442,7 +99442,7 @@
       <c r="F42" s="27">
         <v>0</v>
       </c>
-      <c r="G42" s="29"/>
+      <c r="G42" s="30"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -99520,7 +99520,7 @@
       <c r="F45" s="27">
         <v>0</v>
       </c>
-      <c r="G45" s="29" t="str">
+      <c r="G45" s="30" t="str">
         <f>VLOOKUP(A45,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Other</v>
       </c>
@@ -99546,7 +99546,7 @@
       <c r="F46" s="27">
         <v>0</v>
       </c>
-      <c r="G46" s="29"/>
+      <c r="G46" s="30"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -99570,7 +99570,7 @@
       <c r="F47" s="27">
         <v>0</v>
       </c>
-      <c r="G47" s="29"/>
+      <c r="G47" s="30"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
@@ -99593,7 +99593,7 @@
       <c r="F48" s="27">
         <v>0</v>
       </c>
-      <c r="G48" s="29"/>
+      <c r="G48" s="30"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
@@ -99616,7 +99616,7 @@
       <c r="F49" s="27">
         <v>0</v>
       </c>
-      <c r="G49" s="29"/>
+      <c r="G49" s="30"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="27" t="s">
@@ -100015,7 +100015,7 @@
       <c r="F64" s="27">
         <v>0</v>
       </c>
-      <c r="G64" s="29" t="str">
+      <c r="G64" s="30" t="str">
         <f>VLOOKUP(A64,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100041,7 +100041,7 @@
       <c r="F65" s="27">
         <v>0</v>
       </c>
-      <c r="G65" s="29"/>
+      <c r="G65" s="30"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
@@ -100064,7 +100064,7 @@
       <c r="F66" s="27">
         <v>0</v>
       </c>
-      <c r="G66" s="29" t="str">
+      <c r="G66" s="30" t="str">
         <f>VLOOKUP(A66,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100091,7 +100091,7 @@
       <c r="F67" s="27">
         <v>0</v>
       </c>
-      <c r="G67" s="29"/>
+      <c r="G67" s="30"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
@@ -100114,7 +100114,7 @@
       <c r="F68" s="27">
         <v>0</v>
       </c>
-      <c r="G68" s="29"/>
+      <c r="G68" s="30"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="27" t="s">
@@ -100137,7 +100137,7 @@
       <c r="F69" s="27">
         <v>0</v>
       </c>
-      <c r="G69" s="29" t="str">
+      <c r="G69" s="30" t="str">
         <f>VLOOKUP(A69,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100163,7 +100163,7 @@
       <c r="F70" s="27">
         <v>0</v>
       </c>
-      <c r="G70" s="29"/>
+      <c r="G70" s="30"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -100186,7 +100186,7 @@
       <c r="F71" s="27">
         <v>0</v>
       </c>
-      <c r="G71" s="29" t="str">
+      <c r="G71" s="30" t="str">
         <f>VLOOKUP(A71,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100212,7 +100212,7 @@
       <c r="F72" s="27">
         <v>0</v>
       </c>
-      <c r="G72" s="29"/>
+      <c r="G72" s="30"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="27" t="s">
@@ -100262,7 +100262,7 @@
       <c r="F74" s="27">
         <v>0</v>
       </c>
-      <c r="G74" s="29" t="str">
+      <c r="G74" s="30" t="str">
         <f>VLOOKUP(A74,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100288,7 +100288,7 @@
       <c r="F75" s="27">
         <v>0</v>
       </c>
-      <c r="G75" s="29"/>
+      <c r="G75" s="30"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="27" t="s">
@@ -100311,7 +100311,7 @@
       <c r="F76" s="27">
         <v>0</v>
       </c>
-      <c r="G76" s="29" t="str">
+      <c r="G76" s="30" t="str">
         <f>VLOOKUP(A76,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100337,7 +100337,7 @@
       <c r="F77" s="27">
         <v>0</v>
       </c>
-      <c r="G77" s="29"/>
+      <c r="G77" s="30"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
@@ -100360,7 +100360,7 @@
       <c r="F78" s="27">
         <v>0</v>
       </c>
-      <c r="G78" s="29" t="str">
+      <c r="G78" s="30" t="str">
         <f>VLOOKUP(A78,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100386,7 +100386,7 @@
       <c r="F79" s="27">
         <v>0</v>
       </c>
-      <c r="G79" s="29"/>
+      <c r="G79" s="30"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="27" t="s">
@@ -100409,7 +100409,7 @@
       <c r="F80" s="27">
         <v>0</v>
       </c>
-      <c r="G80" s="29" t="str">
+      <c r="G80" s="30" t="str">
         <f>VLOOKUP(A80,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100435,7 +100435,7 @@
       <c r="F81" s="27">
         <v>0</v>
       </c>
-      <c r="G81" s="29"/>
+      <c r="G81" s="30"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
@@ -100537,7 +100537,7 @@
       <c r="F85" s="27">
         <v>0</v>
       </c>
-      <c r="G85" s="29" t="str">
+      <c r="G85" s="30" t="str">
         <f>VLOOKUP(A85,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Central Metabolism</v>
       </c>
@@ -100564,7 +100564,7 @@
       <c r="F86" s="27">
         <v>0</v>
       </c>
-      <c r="G86" s="29"/>
+      <c r="G86" s="30"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="27" t="s">
@@ -100588,7 +100588,7 @@
       <c r="F87" s="27">
         <v>0</v>
       </c>
-      <c r="G87" s="29"/>
+      <c r="G87" s="30"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
@@ -100612,7 +100612,7 @@
       <c r="F88" s="27">
         <v>0</v>
       </c>
-      <c r="G88" s="29" t="str">
+      <c r="G88" s="30" t="str">
         <f>VLOOKUP(A88,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Antioxidants</v>
       </c>
@@ -100639,7 +100639,7 @@
       <c r="F89" s="27">
         <v>0</v>
       </c>
-      <c r="G89" s="29"/>
+      <c r="G89" s="30"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
@@ -100662,7 +100662,7 @@
       <c r="F90" s="27">
         <v>0</v>
       </c>
-      <c r="G90" s="29"/>
+      <c r="G90" s="30"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
@@ -100685,7 +100685,7 @@
       <c r="F91" s="27">
         <v>0</v>
       </c>
-      <c r="G91" s="29"/>
+      <c r="G91" s="30"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
@@ -100708,7 +100708,7 @@
       <c r="F92" s="27">
         <v>0</v>
       </c>
-      <c r="G92" s="29"/>
+      <c r="G92" s="30"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
@@ -100732,7 +100732,7 @@
       <c r="F93" s="27">
         <v>0</v>
       </c>
-      <c r="G93" s="29"/>
+      <c r="G93" s="30"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
@@ -100755,7 +100755,7 @@
       <c r="F94" s="27">
         <v>0</v>
       </c>
-      <c r="G94" s="29"/>
+      <c r="G94" s="30"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="27" t="s">
@@ -100779,7 +100779,7 @@
       <c r="F95" s="27">
         <v>0</v>
       </c>
-      <c r="G95" s="29" t="str">
+      <c r="G95" s="30" t="str">
         <f>VLOOKUP(A95,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Amino Acid Metabolism</v>
       </c>
@@ -100806,7 +100806,7 @@
       <c r="F96" s="27">
         <v>0</v>
       </c>
-      <c r="G96" s="29"/>
+      <c r="G96" s="30"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
@@ -100830,7 +100830,7 @@
       <c r="F97" s="27">
         <v>0</v>
       </c>
-      <c r="G97" s="29" t="str">
+      <c r="G97" s="30" t="str">
         <f>VLOOKUP(A97,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Other</v>
       </c>
@@ -100857,7 +100857,7 @@
       <c r="F98" s="27">
         <v>0</v>
       </c>
-      <c r="G98" s="29"/>
+      <c r="G98" s="30"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
@@ -100881,7 +100881,7 @@
       <c r="F99" s="27">
         <v>0</v>
       </c>
-      <c r="G99" s="29"/>
+      <c r="G99" s="30"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="27" t="s">
@@ -100932,7 +100932,7 @@
       <c r="F101" s="27">
         <v>0</v>
       </c>
-      <c r="G101" s="29" t="str">
+      <c r="G101" s="30" t="str">
         <f>VLOOKUP(A101,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Amino Acid Metabolism</v>
       </c>
@@ -100959,7 +100959,7 @@
       <c r="F102" s="27">
         <v>0</v>
       </c>
-      <c r="G102" s="29"/>
+      <c r="G102" s="30"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="27" t="s">
@@ -100983,7 +100983,7 @@
       <c r="F103" s="27">
         <v>0</v>
       </c>
-      <c r="G103" s="29" t="str">
+      <c r="G103" s="30" t="str">
         <f>VLOOKUP(A103,Analytical_Standards!$C$2:$K$161,9,FALSE)</f>
         <v>Other</v>
       </c>
@@ -101010,7 +101010,7 @@
       <c r="F104" s="27">
         <v>0</v>
       </c>
-      <c r="G104" s="29"/>
+      <c r="G104" s="30"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F105">
@@ -101020,16 +101020,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="G97:G99"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="G76:G77"/>
-    <mergeCell ref="G78:G79"/>
-    <mergeCell ref="G80:G81"/>
-    <mergeCell ref="G85:G87"/>
-    <mergeCell ref="G88:G94"/>
-    <mergeCell ref="G95:G96"/>
     <mergeCell ref="G101:G102"/>
     <mergeCell ref="G103:G104"/>
     <mergeCell ref="G5:G6"/>
@@ -101046,6 +101036,16 @@
     <mergeCell ref="G41:G42"/>
     <mergeCell ref="G45:G49"/>
     <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="G97:G99"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="G80:G81"/>
+    <mergeCell ref="G85:G87"/>
+    <mergeCell ref="G88:G94"/>
+    <mergeCell ref="G95:G96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>